<commit_message>
memperbaiki view show item
</commit_message>
<xml_diff>
--- a/public/format_data_barang.xlsx
+++ b/public/format_data_barang.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\KEMENKES\APK INVENTORY\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mfahm\Documents\GitHub\gudang-percetakan-negara\public\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5029FEB1-09F2-4519-97CD-86D2D5211234}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE46FEE6-1AC3-4711-9EEB-4761F37E67F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{47EB2AB0-D024-4E86-A293-DC07845C32DA}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>JENIS BARANG</t>
   </si>
@@ -57,6 +57,9 @@
   </si>
   <si>
     <t>PENYIMPANAN BARANG DI GUDANG PN KEMENKES RI</t>
+  </si>
+  <si>
+    <t>KONDISI</t>
   </si>
 </sst>
 </file>
@@ -113,15 +116,19 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -436,10 +443,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C343B087-3D0A-4612-AA6B-4228AB14774E}">
-  <dimension ref="A1:G31"/>
+  <dimension ref="A1:H31"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="J7" sqref="J7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -453,300 +460,304 @@
     <col min="7" max="7" width="13.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:8" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
-      <c r="G1" s="1"/>
-    </row>
-    <row r="2" spans="1:7" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="2" t="s">
+      <c r="B1" s="3"/>
+      <c r="C1" s="3"/>
+      <c r="D1" s="3"/>
+      <c r="E1" s="3"/>
+      <c r="F1" s="3"/>
+      <c r="G1" s="3"/>
+      <c r="H1" s="2"/>
+    </row>
+    <row r="2" spans="1:8" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="D2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="E2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="F2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G2" s="2" t="s">
+      <c r="G2" s="1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A3" s="3"/>
-      <c r="B3" s="3"/>
-      <c r="C3" s="3"/>
-      <c r="D3" s="3"/>
-      <c r="E3" s="3"/>
-      <c r="F3" s="3"/>
-      <c r="G3" s="3"/>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A4" s="3"/>
-      <c r="B4" s="3"/>
-      <c r="C4" s="3"/>
-      <c r="D4" s="3"/>
-      <c r="E4" s="3"/>
-      <c r="F4" s="3"/>
-      <c r="G4" s="3"/>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A5" s="3"/>
-      <c r="B5" s="3"/>
-      <c r="C5" s="3"/>
-      <c r="D5" s="3"/>
-      <c r="E5" s="3"/>
-      <c r="F5" s="3"/>
-      <c r="G5" s="3"/>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A6" s="3"/>
-      <c r="B6" s="3"/>
-      <c r="C6" s="3"/>
-      <c r="D6" s="3"/>
-      <c r="E6" s="3"/>
-      <c r="F6" s="3"/>
-      <c r="G6" s="3"/>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A7" s="3"/>
-      <c r="B7" s="3"/>
-      <c r="C7" s="3"/>
-      <c r="D7" s="3"/>
-      <c r="E7" s="3"/>
-      <c r="F7" s="3"/>
-      <c r="G7" s="3"/>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A8" s="3"/>
-      <c r="B8" s="3"/>
-      <c r="C8" s="3"/>
-      <c r="D8" s="3"/>
-      <c r="E8" s="3"/>
-      <c r="F8" s="3"/>
-      <c r="G8" s="3"/>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A9" s="3"/>
-      <c r="B9" s="3"/>
-      <c r="C9" s="3"/>
-      <c r="D9" s="3"/>
-      <c r="E9" s="3"/>
-      <c r="F9" s="3"/>
-      <c r="G9" s="3"/>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A10" s="3"/>
-      <c r="B10" s="3"/>
-      <c r="C10" s="3"/>
-      <c r="D10" s="3"/>
-      <c r="E10" s="3"/>
-      <c r="F10" s="3"/>
-      <c r="G10" s="3"/>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A11" s="3"/>
-      <c r="B11" s="3"/>
-      <c r="C11" s="3"/>
-      <c r="D11" s="3"/>
-      <c r="E11" s="3"/>
-      <c r="F11" s="3"/>
-      <c r="G11" s="3"/>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A12" s="3"/>
-      <c r="B12" s="3"/>
-      <c r="C12" s="3"/>
-      <c r="D12" s="3"/>
-      <c r="E12" s="3"/>
-      <c r="F12" s="3"/>
-      <c r="G12" s="3"/>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A13" s="3"/>
-      <c r="B13" s="3"/>
-      <c r="C13" s="3"/>
-      <c r="D13" s="3"/>
-      <c r="E13" s="3"/>
-      <c r="F13" s="3"/>
-      <c r="G13" s="3"/>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A14" s="3"/>
-      <c r="B14" s="3"/>
-      <c r="C14" s="3"/>
-      <c r="D14" s="3"/>
-      <c r="E14" s="3"/>
-      <c r="F14" s="3"/>
-      <c r="G14" s="3"/>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A15" s="3"/>
-      <c r="B15" s="3"/>
-      <c r="C15" s="3"/>
-      <c r="D15" s="3"/>
-      <c r="E15" s="3"/>
-      <c r="F15" s="3"/>
-      <c r="G15" s="3"/>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A16" s="3"/>
-      <c r="B16" s="3"/>
-      <c r="C16" s="3"/>
-      <c r="D16" s="3"/>
-      <c r="E16" s="3"/>
-      <c r="F16" s="3"/>
-      <c r="G16" s="3"/>
+      <c r="H2" s="5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A3" s="4"/>
+      <c r="B3" s="4"/>
+      <c r="C3" s="4"/>
+      <c r="D3" s="4"/>
+      <c r="E3" s="4"/>
+      <c r="F3" s="4"/>
+      <c r="G3" s="4"/>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A4" s="4"/>
+      <c r="B4" s="4"/>
+      <c r="C4" s="4"/>
+      <c r="D4" s="4"/>
+      <c r="E4" s="4"/>
+      <c r="F4" s="4"/>
+      <c r="G4" s="4"/>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A5" s="4"/>
+      <c r="B5" s="4"/>
+      <c r="C5" s="4"/>
+      <c r="D5" s="4"/>
+      <c r="E5" s="4"/>
+      <c r="F5" s="4"/>
+      <c r="G5" s="4"/>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A6" s="4"/>
+      <c r="B6" s="4"/>
+      <c r="C6" s="4"/>
+      <c r="D6" s="4"/>
+      <c r="E6" s="4"/>
+      <c r="F6" s="4"/>
+      <c r="G6" s="4"/>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A7" s="4"/>
+      <c r="B7" s="4"/>
+      <c r="C7" s="4"/>
+      <c r="D7" s="4"/>
+      <c r="E7" s="4"/>
+      <c r="F7" s="4"/>
+      <c r="G7" s="4"/>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A8" s="4"/>
+      <c r="B8" s="4"/>
+      <c r="C8" s="4"/>
+      <c r="D8" s="4"/>
+      <c r="E8" s="4"/>
+      <c r="F8" s="4"/>
+      <c r="G8" s="4"/>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A9" s="4"/>
+      <c r="B9" s="4"/>
+      <c r="C9" s="4"/>
+      <c r="D9" s="4"/>
+      <c r="E9" s="4"/>
+      <c r="F9" s="4"/>
+      <c r="G9" s="4"/>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A10" s="4"/>
+      <c r="B10" s="4"/>
+      <c r="C10" s="4"/>
+      <c r="D10" s="4"/>
+      <c r="E10" s="4"/>
+      <c r="F10" s="4"/>
+      <c r="G10" s="4"/>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A11" s="4"/>
+      <c r="B11" s="4"/>
+      <c r="C11" s="4"/>
+      <c r="D11" s="4"/>
+      <c r="E11" s="4"/>
+      <c r="F11" s="4"/>
+      <c r="G11" s="4"/>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A12" s="4"/>
+      <c r="B12" s="4"/>
+      <c r="C12" s="4"/>
+      <c r="D12" s="4"/>
+      <c r="E12" s="4"/>
+      <c r="F12" s="4"/>
+      <c r="G12" s="4"/>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A13" s="4"/>
+      <c r="B13" s="4"/>
+      <c r="C13" s="4"/>
+      <c r="D13" s="4"/>
+      <c r="E13" s="4"/>
+      <c r="F13" s="4"/>
+      <c r="G13" s="4"/>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A14" s="4"/>
+      <c r="B14" s="4"/>
+      <c r="C14" s="4"/>
+      <c r="D14" s="4"/>
+      <c r="E14" s="4"/>
+      <c r="F14" s="4"/>
+      <c r="G14" s="4"/>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A15" s="4"/>
+      <c r="B15" s="4"/>
+      <c r="C15" s="4"/>
+      <c r="D15" s="4"/>
+      <c r="E15" s="4"/>
+      <c r="F15" s="4"/>
+      <c r="G15" s="4"/>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A16" s="4"/>
+      <c r="B16" s="4"/>
+      <c r="C16" s="4"/>
+      <c r="D16" s="4"/>
+      <c r="E16" s="4"/>
+      <c r="F16" s="4"/>
+      <c r="G16" s="4"/>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A17" s="3"/>
-      <c r="B17" s="3"/>
-      <c r="C17" s="3"/>
-      <c r="D17" s="3"/>
-      <c r="E17" s="3"/>
-      <c r="F17" s="3"/>
-      <c r="G17" s="3"/>
+      <c r="A17" s="4"/>
+      <c r="B17" s="4"/>
+      <c r="C17" s="4"/>
+      <c r="D17" s="4"/>
+      <c r="E17" s="4"/>
+      <c r="F17" s="4"/>
+      <c r="G17" s="4"/>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A18" s="3"/>
-      <c r="B18" s="3"/>
-      <c r="C18" s="3"/>
-      <c r="D18" s="3"/>
-      <c r="E18" s="3"/>
-      <c r="F18" s="3"/>
-      <c r="G18" s="3"/>
+      <c r="A18" s="4"/>
+      <c r="B18" s="4"/>
+      <c r="C18" s="4"/>
+      <c r="D18" s="4"/>
+      <c r="E18" s="4"/>
+      <c r="F18" s="4"/>
+      <c r="G18" s="4"/>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A19" s="3"/>
-      <c r="B19" s="3"/>
-      <c r="C19" s="3"/>
-      <c r="D19" s="3"/>
-      <c r="E19" s="3"/>
-      <c r="F19" s="3"/>
-      <c r="G19" s="3"/>
+      <c r="A19" s="4"/>
+      <c r="B19" s="4"/>
+      <c r="C19" s="4"/>
+      <c r="D19" s="4"/>
+      <c r="E19" s="4"/>
+      <c r="F19" s="4"/>
+      <c r="G19" s="4"/>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A20" s="3"/>
-      <c r="B20" s="3"/>
-      <c r="C20" s="3"/>
-      <c r="D20" s="3"/>
-      <c r="E20" s="3"/>
-      <c r="F20" s="3"/>
-      <c r="G20" s="3"/>
+      <c r="A20" s="4"/>
+      <c r="B20" s="4"/>
+      <c r="C20" s="4"/>
+      <c r="D20" s="4"/>
+      <c r="E20" s="4"/>
+      <c r="F20" s="4"/>
+      <c r="G20" s="4"/>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A21" s="3"/>
-      <c r="B21" s="3"/>
-      <c r="C21" s="3"/>
-      <c r="D21" s="3"/>
-      <c r="E21" s="3"/>
-      <c r="F21" s="3"/>
-      <c r="G21" s="3"/>
+      <c r="A21" s="4"/>
+      <c r="B21" s="4"/>
+      <c r="C21" s="4"/>
+      <c r="D21" s="4"/>
+      <c r="E21" s="4"/>
+      <c r="F21" s="4"/>
+      <c r="G21" s="4"/>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A22" s="3"/>
-      <c r="B22" s="3"/>
-      <c r="C22" s="3"/>
-      <c r="D22" s="3"/>
-      <c r="E22" s="3"/>
-      <c r="F22" s="3"/>
-      <c r="G22" s="3"/>
+      <c r="A22" s="4"/>
+      <c r="B22" s="4"/>
+      <c r="C22" s="4"/>
+      <c r="D22" s="4"/>
+      <c r="E22" s="4"/>
+      <c r="F22" s="4"/>
+      <c r="G22" s="4"/>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A23" s="3"/>
-      <c r="B23" s="3"/>
-      <c r="C23" s="3"/>
-      <c r="D23" s="3"/>
-      <c r="E23" s="3"/>
-      <c r="F23" s="3"/>
-      <c r="G23" s="3"/>
+      <c r="A23" s="4"/>
+      <c r="B23" s="4"/>
+      <c r="C23" s="4"/>
+      <c r="D23" s="4"/>
+      <c r="E23" s="4"/>
+      <c r="F23" s="4"/>
+      <c r="G23" s="4"/>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A24" s="3"/>
-      <c r="B24" s="3"/>
-      <c r="C24" s="3"/>
-      <c r="D24" s="3"/>
-      <c r="E24" s="3"/>
-      <c r="F24" s="3"/>
-      <c r="G24" s="3"/>
+      <c r="A24" s="4"/>
+      <c r="B24" s="4"/>
+      <c r="C24" s="4"/>
+      <c r="D24" s="4"/>
+      <c r="E24" s="4"/>
+      <c r="F24" s="4"/>
+      <c r="G24" s="4"/>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A25" s="3"/>
-      <c r="B25" s="3"/>
-      <c r="C25" s="3"/>
-      <c r="D25" s="3"/>
-      <c r="E25" s="3"/>
-      <c r="F25" s="3"/>
-      <c r="G25" s="3"/>
+      <c r="A25" s="4"/>
+      <c r="B25" s="4"/>
+      <c r="C25" s="4"/>
+      <c r="D25" s="4"/>
+      <c r="E25" s="4"/>
+      <c r="F25" s="4"/>
+      <c r="G25" s="4"/>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A26" s="3"/>
-      <c r="B26" s="3"/>
-      <c r="C26" s="3"/>
-      <c r="D26" s="3"/>
-      <c r="E26" s="3"/>
-      <c r="F26" s="3"/>
-      <c r="G26" s="3"/>
+      <c r="A26" s="4"/>
+      <c r="B26" s="4"/>
+      <c r="C26" s="4"/>
+      <c r="D26" s="4"/>
+      <c r="E26" s="4"/>
+      <c r="F26" s="4"/>
+      <c r="G26" s="4"/>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A27" s="3"/>
-      <c r="B27" s="3"/>
-      <c r="C27" s="3"/>
-      <c r="D27" s="3"/>
-      <c r="E27" s="3"/>
-      <c r="F27" s="3"/>
-      <c r="G27" s="3"/>
+      <c r="A27" s="4"/>
+      <c r="B27" s="4"/>
+      <c r="C27" s="4"/>
+      <c r="D27" s="4"/>
+      <c r="E27" s="4"/>
+      <c r="F27" s="4"/>
+      <c r="G27" s="4"/>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A28" s="3"/>
-      <c r="B28" s="3"/>
-      <c r="C28" s="3"/>
-      <c r="D28" s="3"/>
-      <c r="E28" s="3"/>
-      <c r="F28" s="3"/>
-      <c r="G28" s="3"/>
+      <c r="A28" s="4"/>
+      <c r="B28" s="4"/>
+      <c r="C28" s="4"/>
+      <c r="D28" s="4"/>
+      <c r="E28" s="4"/>
+      <c r="F28" s="4"/>
+      <c r="G28" s="4"/>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A29" s="3"/>
-      <c r="B29" s="3"/>
-      <c r="C29" s="3"/>
-      <c r="D29" s="3"/>
-      <c r="E29" s="3"/>
-      <c r="F29" s="3"/>
-      <c r="G29" s="3"/>
+      <c r="A29" s="4"/>
+      <c r="B29" s="4"/>
+      <c r="C29" s="4"/>
+      <c r="D29" s="4"/>
+      <c r="E29" s="4"/>
+      <c r="F29" s="4"/>
+      <c r="G29" s="4"/>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A30" s="3"/>
-      <c r="B30" s="3"/>
-      <c r="C30" s="3"/>
-      <c r="D30" s="3"/>
-      <c r="E30" s="3"/>
-      <c r="F30" s="3"/>
-      <c r="G30" s="3"/>
+      <c r="A30" s="4"/>
+      <c r="B30" s="4"/>
+      <c r="C30" s="4"/>
+      <c r="D30" s="4"/>
+      <c r="E30" s="4"/>
+      <c r="F30" s="4"/>
+      <c r="G30" s="4"/>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A31" s="3"/>
-      <c r="B31" s="3"/>
-      <c r="C31" s="3"/>
-      <c r="D31" s="3"/>
-      <c r="E31" s="3"/>
-      <c r="F31" s="3"/>
-      <c r="G31" s="3"/>
+      <c r="A31" s="4"/>
+      <c r="B31" s="4"/>
+      <c r="C31" s="4"/>
+      <c r="D31" s="4"/>
+      <c r="E31" s="4"/>
+      <c r="F31" s="4"/>
+      <c r="G31" s="4"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>